<commit_message>
new changes in form
</commit_message>
<xml_diff>
--- a/src/test/resources/formsautomation.xlsx
+++ b/src/test/resources/formsautomation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>No</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>14-01-2026 16:33:43</t>
+  </si>
+  <si>
+    <t>20-01-2026 15:20:22</t>
   </si>
 </sst>
 </file>
@@ -1888,7 +1891,7 @@
         <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>